<commit_message>
Ajout des liens vers les réseau sociaux dans la page contact et réctification de l'emplacment des images lorsqu'on active l'agrandissement
</commit_message>
<xml_diff>
--- a/Doc/Audit-SEO.xlsx
+++ b/Doc/Audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ISMAIL\Documents\La chouette agence\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451656C2-F479-4748-B6ED-BEA6BA48B138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE5B193-CC3F-444A-A69F-4F0CAA618645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
   <si>
     <t>Catégorie</t>
   </si>
@@ -251,6 +251,30 @@
   </si>
   <si>
     <t>https://blog.lws-hosting.com/referencement-naturel-seo/comment-optimiser-son-site-web-avec-la-minification-css-js-et-html</t>
+  </si>
+  <si>
+    <t>Tous les éléments de la page ne portent pas le focus de manière visible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tous les éléments activables DOIVENT être focusables </t>
+  </si>
+  <si>
+    <t>Tous les éléments activables DOIVENT pouvoir porter le focus </t>
+  </si>
+  <si>
+    <t>https://www.24joursdeweb.fr/2017/le-focus-nest-pas-juste-une-astuce/</t>
+  </si>
+  <si>
+    <t>https://smartkeyword.io/seo-on-page-images-attribut-alt/</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist#focus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Certain champ ne sont pas focus lorsque on les sélectionnes </t>
   </si>
 </sst>
 </file>
@@ -567,16 +591,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z15"/>
+  <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="58.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="65.109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="131.33203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="39.21875" style="3" customWidth="1"/>
     <col min="5" max="5" width="40.88671875" style="3" customWidth="1"/>
@@ -896,6 +920,37 @@
       <c r="E15" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="F15" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="45" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -911,8 +966,11 @@
     <hyperlink ref="F3" r:id="rId10" xr:uid="{EA411016-A6AB-4782-8F18-E8C570F5C3DA}"/>
     <hyperlink ref="F7" r:id="rId11" xr:uid="{8BB6AE27-E4EB-4976-8802-C602DF94E344}"/>
     <hyperlink ref="F13" r:id="rId12" xr:uid="{39F492FB-6B70-4506-9FCC-9CD72134ED0C}"/>
+    <hyperlink ref="F16" r:id="rId13" xr:uid="{707626BD-1E87-4D22-BA45-E5C3A851EDC4}"/>
+    <hyperlink ref="F15" r:id="rId14" xr:uid="{FDC6CCC2-44BF-4591-9C8E-678014865B1C}"/>
+    <hyperlink ref="B19" r:id="rId15" location="focus" xr:uid="{AC142342-D06F-4027-8993-43326903AC07}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId13"/>
+  <pageSetup orientation="landscape" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>